<commit_message>
Backend/codegen: 通过 xpl 函数 GenOrmModelExtAttrs 统一构造 OrmModel 的扩展属性，并以 OrmModel 为构建 Maven 模块工程代码的数据模型
</commit_message>
<xml_diff>
--- a/code/backend/010.codegen/model/duzhou-app-modeler.app-module.xlsx
+++ b/code/backend/010.codegen/model/duzhou-app-modeler.app-module.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27645" windowHeight="12330" activeTab="4"/>
+    <workbookView windowWidth="27645" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="配置" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>duzhou-platform</t>
   </si>
   <si>
-    <t>app.name</t>
+    <t>app.displayName</t>
   </si>
   <si>
     <t>渡舟平台</t>
@@ -118,7 +118,7 @@
     <t>可选值：spring, quarkus</t>
   </si>
   <si>
-    <t>app.module.name</t>
+    <t>app.module.displayName</t>
   </si>
   <si>
     <t>应用建模器</t>
@@ -2489,8 +2489,8 @@
   <sheetPr/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.125" defaultRowHeight="16.5" outlineLevelCol="2"/>
@@ -4152,7 +4152,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -6465,7 +6465,7 @@
   <sheetPr/>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -8937,8 +8937,8 @@
   <sheetPr/>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:O33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>